<commit_message>
tweak address book validation
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="227670" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="231390" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1949" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1939" uniqueCount="586">
   <si>
     <t>Please enter a first name</t>
   </si>
@@ -694,9 +694,6 @@
     <t>U77</t>
   </si>
   <si>
-    <t>add new  address</t>
-  </si>
-  <si>
     <t>edit address</t>
   </si>
   <si>
@@ -829,12 +826,6 @@
     <t>A4</t>
   </si>
   <si>
-    <t>update default payment</t>
-  </si>
-  <si>
-    <t>delete payment</t>
-  </si>
-  <si>
     <t>fieldsValidation</t>
   </si>
   <si>
@@ -887,12 +878,6 @@
   </si>
   <si>
     <t>tester1@ordershistory.com</t>
-  </si>
-  <si>
-    <t>Add a new payment through checkout and update the default payment</t>
-  </si>
-  <si>
-    <t>Add a new payment through checkout then delete it from payment page</t>
   </si>
   <si>
     <t xml:space="preserve">Guest, verify the PDP basics </t>
@@ -1869,6 +1854,28 @@
   </si>
   <si>
     <t>newQty</t>
+  </si>
+  <si>
+    <t>Add Payment method with spesific address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Payment </t>
+  </si>
+  <si>
+    <t>add new  address
+delete address</t>
+  </si>
+  <si>
+    <t>proprites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add address and remove it </t>
+  </si>
+  <si>
+    <t>add new  address
+default Address
+edit address
+delete address</t>
   </si>
 </sst>
 </file>
@@ -2736,7 +2743,7 @@
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1">
       <c r="A2" s="18" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="22" t="s">
@@ -2755,12 +2762,12 @@
         <v>44</v>
       </c>
       <c r="H2" s="69" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1">
       <c r="A3" s="18" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="22" t="s">
@@ -2779,12 +2786,12 @@
         <v>45</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1">
       <c r="A4" s="18" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="22" t="s">
@@ -2803,12 +2810,12 @@
         <v>44</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1">
       <c r="A5" s="18" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B5" s="18"/>
       <c r="C5" s="22" t="s">
@@ -2827,12 +2834,12 @@
         <v>44</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1">
       <c r="A6" s="18" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="22" t="s">
@@ -2851,12 +2858,12 @@
         <v>45</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1">
       <c r="A7" s="18" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="22" t="s">
@@ -2875,12 +2882,12 @@
         <v>44</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1">
       <c r="A8" s="18" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="22" t="s">
@@ -2899,12 +2906,12 @@
         <v>44</v>
       </c>
       <c r="H8" s="33" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1">
       <c r="A9" s="18" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="22" t="s">
@@ -2923,12 +2930,12 @@
         <v>45</v>
       </c>
       <c r="H9" s="33" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1">
       <c r="A10" s="18" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="22" t="s">
@@ -2947,12 +2954,12 @@
         <v>44</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1">
       <c r="A11" s="18" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="22" t="s">
@@ -2971,12 +2978,12 @@
         <v>44</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="18" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="22" t="s">
@@ -2995,12 +3002,12 @@
         <v>45</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="18" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="22" t="s">
@@ -3019,12 +3026,12 @@
         <v>44</v>
       </c>
       <c r="H13" s="33" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="22" t="s">
@@ -3043,12 +3050,12 @@
         <v>44</v>
       </c>
       <c r="H14" s="33" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="18" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="22" t="s">
@@ -3067,12 +3074,12 @@
         <v>45</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="18" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="22" t="s">
@@ -3091,12 +3098,12 @@
         <v>44</v>
       </c>
       <c r="H16" s="33" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="18" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="22" t="s">
@@ -3115,12 +3122,12 @@
         <v>44</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="18" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="22" t="s">
@@ -3139,12 +3146,12 @@
         <v>45</v>
       </c>
       <c r="H18" s="33" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="18" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="22" t="s">
@@ -3163,12 +3170,12 @@
         <v>44</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="18" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="22" t="s">
@@ -3187,12 +3194,12 @@
         <v>44</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="18" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="22" t="s">
@@ -3211,12 +3218,12 @@
         <v>45</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="18" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="22" t="s">
@@ -3235,12 +3242,12 @@
         <v>44</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="18" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="22" t="s">
@@ -3259,12 +3266,12 @@
         <v>44</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="18" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="22" t="s">
@@ -3283,12 +3290,12 @@
         <v>45</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="18" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="22" t="s">
@@ -3307,12 +3314,12 @@
         <v>44</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="18" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="22" t="s">
@@ -3331,12 +3338,12 @@
         <v>44</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="18" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="22" t="s">
@@ -3355,12 +3362,12 @@
         <v>45</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="22" t="s">
@@ -3379,12 +3386,12 @@
         <v>44</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="18" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="22" t="s">
@@ -3403,12 +3410,12 @@
         <v>44</v>
       </c>
       <c r="H29" s="33" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="22" t="s">
@@ -3427,12 +3434,12 @@
         <v>45</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="18" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="22" t="s">
@@ -3451,12 +3458,12 @@
         <v>44</v>
       </c>
       <c r="H31" s="33" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="22" t="s">
@@ -3475,12 +3482,12 @@
         <v>44</v>
       </c>
       <c r="H32" s="33" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="18" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="22" t="s">
@@ -3499,12 +3506,12 @@
         <v>45</v>
       </c>
       <c r="H33" s="33" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="22" t="s">
@@ -3523,12 +3530,12 @@
         <v>44</v>
       </c>
       <c r="H34" s="33" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="18" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="22" t="s">
@@ -3547,12 +3554,12 @@
         <v>44</v>
       </c>
       <c r="H35" s="33" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="18" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="22" t="s">
@@ -3571,12 +3578,12 @@
         <v>45</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="18" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="22" t="s">
@@ -3595,12 +3602,12 @@
         <v>44</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="18" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="22" t="s">
@@ -3619,12 +3626,12 @@
         <v>44</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="18" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B39" s="18" t="s">
         <v>57</v>
@@ -3645,12 +3652,12 @@
         <v>44</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="18" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="22" t="s">
@@ -3669,12 +3676,12 @@
         <v>44</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="18" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="22" t="s">
@@ -3693,12 +3700,12 @@
         <v>44</v>
       </c>
       <c r="H41" s="72" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="18" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="22" t="s">
@@ -3717,12 +3724,12 @@
         <v>44</v>
       </c>
       <c r="H42" s="32" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="18" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="22" t="s">
@@ -3741,12 +3748,12 @@
         <v>44</v>
       </c>
       <c r="H43" s="32" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="18" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="22" t="s">
@@ -3765,12 +3772,12 @@
         <v>44</v>
       </c>
       <c r="H44" s="32" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="18" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="22" t="s">
@@ -3789,12 +3796,12 @@
         <v>44</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="18" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="B46" s="18"/>
       <c r="C46" s="22" t="s">
@@ -3813,12 +3820,12 @@
         <v>44</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="18" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B47" s="18"/>
       <c r="C47" s="22" t="s">
@@ -3837,12 +3844,12 @@
         <v>44</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="18" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B48" s="18"/>
       <c r="C48" s="22" t="s">
@@ -3861,7 +3868,7 @@
         <v>44</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -3914,69 +3921,69 @@
         <v>15</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>218</v>
-      </c>
       <c r="K1" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="L1" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="M1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="P1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="2" spans="4:20" ht="45">
       <c r="D2" s="37" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>57</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="K2" s="39">
         <v>1</v>
@@ -3985,7 +3992,7 @@
         <v>3</v>
       </c>
       <c r="M2" s="40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N2" s="41">
         <v>3</v>
@@ -4011,25 +4018,25 @@
     </row>
     <row r="3" spans="4:20" ht="45">
       <c r="D3" s="37" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="K3" s="38">
         <v>1</v>
@@ -4038,7 +4045,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N3" s="41">
         <v>2</v>
@@ -4064,25 +4071,25 @@
     </row>
     <row r="4" spans="4:20" ht="30">
       <c r="D4" s="37" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="E4" s="37" t="s">
         <v>57</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K4" s="38">
         <v>1</v>
@@ -4091,7 +4098,7 @@
         <v>1</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N4" s="41">
         <v>1</v>
@@ -4117,25 +4124,25 @@
     </row>
     <row r="5" spans="4:20" ht="45">
       <c r="D5" s="37" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E5" s="37" t="s">
         <v>57</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K5" s="38">
         <v>2</v>
@@ -4170,16 +4177,16 @@
     </row>
     <row r="6" spans="4:20" ht="30">
       <c r="D6" s="37" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>57</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -4256,7 +4263,7 @@
         <v>47</v>
       </c>
       <c r="J1" s="63" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K1" s="31" t="s">
         <v>124</v>
@@ -4270,10 +4277,10 @@
         <v>57</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D2" s="61" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E2" s="62" t="s">
         <v>4</v>
@@ -4291,10 +4298,10 @@
         <v>44</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -4305,10 +4312,10 @@
         <v>57</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E3" s="62" t="s">
         <v>4</v>
@@ -4326,10 +4333,10 @@
         <v>44</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K3" s="54" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60">
@@ -4340,10 +4347,10 @@
         <v>57</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E4" s="62" t="s">
         <v>4</v>
@@ -4361,7 +4368,7 @@
         <v>44</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K4" s="54" t="s">
         <v>0</v>
@@ -4375,10 +4382,10 @@
         <v>57</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E5" s="62" t="s">
         <v>4</v>
@@ -4396,7 +4403,7 @@
         <v>44</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K5" s="54" t="s">
         <v>1</v>
@@ -4410,10 +4417,10 @@
         <v>57</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E6" s="62" t="s">
         <v>4</v>
@@ -4431,10 +4438,10 @@
         <v>44</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60">
@@ -4445,10 +4452,10 @@
         <v>57</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E7" s="62" t="s">
         <v>4</v>
@@ -4466,10 +4473,10 @@
         <v>44</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60">
@@ -4480,10 +4487,10 @@
         <v>57</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E8" s="62" t="s">
         <v>4</v>
@@ -4501,10 +4508,10 @@
         <v>44</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45">
@@ -4515,10 +4522,10 @@
         <v>57</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>4</v>
@@ -4530,16 +4537,16 @@
         <v>16</v>
       </c>
       <c r="H9" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I9" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45">
@@ -4550,10 +4557,10 @@
         <v>57</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E10" s="62" t="s">
         <v>4</v>
@@ -4565,16 +4572,16 @@
         <v>16</v>
       </c>
       <c r="H10" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I10" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K10" s="26" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45">
@@ -4585,10 +4592,10 @@
         <v>57</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E11" s="62" t="s">
         <v>4</v>
@@ -4600,16 +4607,16 @@
         <v>16</v>
       </c>
       <c r="H11" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I11" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J11" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K11" s="26" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45">
@@ -4620,10 +4627,10 @@
         <v>57</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E12" s="62" t="s">
         <v>4</v>
@@ -4635,16 +4642,16 @@
         <v>16</v>
       </c>
       <c r="H12" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I12" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K12" s="26" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45">
@@ -4655,10 +4662,10 @@
         <v>57</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E13" s="62" t="s">
         <v>4</v>
@@ -4670,16 +4677,16 @@
         <v>16</v>
       </c>
       <c r="H13" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I13" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J13" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="K13" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="K13" s="26" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45">
@@ -4690,10 +4697,10 @@
         <v>57</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E14" s="62" t="s">
         <v>4</v>
@@ -4705,16 +4712,16 @@
         <v>16</v>
       </c>
       <c r="H14" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I14" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J14" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="45">
@@ -4725,10 +4732,10 @@
         <v>57</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E15" s="62" t="s">
         <v>4</v>
@@ -4740,16 +4747,16 @@
         <v>16</v>
       </c>
       <c r="H15" s="61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I15" s="61" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -4795,103 +4802,103 @@
         <v>13</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="47" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D2" s="70" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="47" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D3" s="70" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="47" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="D4" s="70" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>150</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="47" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="B5" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="E5" s="32" t="s">
         <v>150</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="47" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D6" s="70" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E6" s="70"/>
       <c r="F6" s="80" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -4950,7 +4957,7 @@
         <v>69</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>2</v>
@@ -4962,7 +4969,7 @@
         <v>91</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4973,7 +4980,7 @@
         <v>69</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>2</v>
@@ -4996,7 +5003,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>2</v>
@@ -5019,7 +5026,7 @@
         <v>69</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>2</v>
@@ -5042,7 +5049,7 @@
         <v>69</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>2</v>
@@ -5065,7 +5072,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>2</v>
@@ -5088,7 +5095,7 @@
         <v>69</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>2</v>
@@ -5111,7 +5118,7 @@
         <v>69</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>2</v>
@@ -5134,7 +5141,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>2</v>
@@ -5157,7 +5164,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>2</v>
@@ -5180,7 +5187,7 @@
         <v>69</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>2</v>
@@ -5203,7 +5210,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>2</v>
@@ -5226,7 +5233,7 @@
         <v>69</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>2</v>
@@ -5249,7 +5256,7 @@
         <v>69</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>2</v>
@@ -5272,7 +5279,7 @@
         <v>69</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>2</v>
@@ -5295,7 +5302,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>2</v>
@@ -5318,7 +5325,7 @@
         <v>69</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>2</v>
@@ -5341,7 +5348,7 @@
         <v>69</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D19" s="29" t="s">
         <v>2</v>
@@ -5364,7 +5371,7 @@
         <v>69</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D20" s="29" t="s">
         <v>2</v>
@@ -5387,7 +5394,7 @@
         <v>69</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D21" s="29" t="s">
         <v>2</v>
@@ -5410,7 +5417,7 @@
         <v>69</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D22" s="29" t="s">
         <v>2</v>
@@ -5433,7 +5440,7 @@
         <v>69</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D23" s="29" t="s">
         <v>2</v>
@@ -5456,7 +5463,7 @@
         <v>69</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D24" s="29" t="s">
         <v>2</v>
@@ -5479,7 +5486,7 @@
         <v>69</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>2</v>
@@ -5502,7 +5509,7 @@
         <v>69</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D26" s="29" t="s">
         <v>2</v>
@@ -5525,7 +5532,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>2</v>
@@ -5537,7 +5544,7 @@
         <v>91</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5548,7 +5555,7 @@
         <v>69</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D28" s="29" t="s">
         <v>2</v>
@@ -5560,7 +5567,7 @@
         <v>91</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -5571,7 +5578,7 @@
         <v>69</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>2</v>
@@ -5583,7 +5590,7 @@
         <v>91</v>
       </c>
       <c r="G29" s="69" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5594,7 +5601,7 @@
         <v>69</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D30" s="29" t="s">
         <v>2</v>
@@ -5606,7 +5613,7 @@
         <v>91</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5617,7 +5624,7 @@
         <v>69</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D31" s="29" t="s">
         <v>2</v>
@@ -5629,7 +5636,7 @@
         <v>91</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5640,7 +5647,7 @@
         <v>69</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>2</v>
@@ -5652,7 +5659,7 @@
         <v>91</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5663,7 +5670,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D33" s="29" t="s">
         <v>2</v>
@@ -5675,7 +5682,7 @@
         <v>91</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5686,7 +5693,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D34" s="29" t="s">
         <v>2</v>
@@ -5698,7 +5705,7 @@
         <v>91</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5709,7 +5716,7 @@
         <v>69</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D35" s="29" t="s">
         <v>2</v>
@@ -5721,7 +5728,7 @@
         <v>91</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5732,7 +5739,7 @@
         <v>69</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D36" s="29" t="s">
         <v>2</v>
@@ -5744,7 +5751,7 @@
         <v>91</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5755,7 +5762,7 @@
         <v>69</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>2</v>
@@ -5767,7 +5774,7 @@
         <v>91</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5778,7 +5785,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D38" s="29" t="s">
         <v>2</v>
@@ -5790,7 +5797,7 @@
         <v>91</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -5801,7 +5808,7 @@
         <v>69</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D39" s="29" t="s">
         <v>2</v>
@@ -5813,7 +5820,7 @@
         <v>91</v>
       </c>
       <c r="G39" s="33" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -5824,7 +5831,7 @@
         <v>69</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D40" s="29" t="s">
         <v>2</v>
@@ -5836,7 +5843,7 @@
         <v>91</v>
       </c>
       <c r="G40" s="33" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -5847,7 +5854,7 @@
         <v>69</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D41" s="29" t="s">
         <v>2</v>
@@ -5859,7 +5866,7 @@
         <v>91</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -5870,7 +5877,7 @@
         <v>69</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D42" s="29" t="s">
         <v>2</v>
@@ -5882,7 +5889,7 @@
         <v>91</v>
       </c>
       <c r="G42" s="33" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -5893,7 +5900,7 @@
         <v>69</v>
       </c>
       <c r="C43" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D43" s="29" t="s">
         <v>2</v>
@@ -5905,7 +5912,7 @@
         <v>91</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -5916,7 +5923,7 @@
         <v>69</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D44" s="29" t="s">
         <v>2</v>
@@ -5928,7 +5935,7 @@
         <v>91</v>
       </c>
       <c r="G44" s="33" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -5939,7 +5946,7 @@
         <v>69</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D45" s="29" t="s">
         <v>2</v>
@@ -5951,7 +5958,7 @@
         <v>91</v>
       </c>
       <c r="G45" s="33" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -5962,7 +5969,7 @@
         <v>69</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D46" s="29" t="s">
         <v>2</v>
@@ -5974,7 +5981,7 @@
         <v>91</v>
       </c>
       <c r="G46" s="33" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -5985,7 +5992,7 @@
         <v>69</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D47" s="29" t="s">
         <v>2</v>
@@ -5997,7 +6004,7 @@
         <v>91</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -6008,7 +6015,7 @@
         <v>69</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D48" s="29" t="s">
         <v>2</v>
@@ -6020,7 +6027,7 @@
         <v>91</v>
       </c>
       <c r="G48" s="33" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -6031,7 +6038,7 @@
         <v>69</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D49" s="29" t="s">
         <v>2</v>
@@ -6043,7 +6050,7 @@
         <v>91</v>
       </c>
       <c r="G49" s="33" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -6054,7 +6061,7 @@
         <v>69</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D50" s="29" t="s">
         <v>2</v>
@@ -6066,7 +6073,7 @@
         <v>91</v>
       </c>
       <c r="G50" s="33" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -6077,7 +6084,7 @@
         <v>69</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D51" s="29" t="s">
         <v>2</v>
@@ -6089,7 +6096,7 @@
         <v>91</v>
       </c>
       <c r="G51" s="33" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -6100,7 +6107,7 @@
         <v>69</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D52" s="29" t="s">
         <v>2</v>
@@ -6112,7 +6119,7 @@
         <v>91</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -6123,7 +6130,7 @@
         <v>69</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D53" s="29" t="s">
         <v>2</v>
@@ -6135,7 +6142,7 @@
         <v>91</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -6146,7 +6153,7 @@
         <v>69</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D54" s="29" t="s">
         <v>2</v>
@@ -6158,7 +6165,7 @@
         <v>91</v>
       </c>
       <c r="G54" s="33" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -6169,7 +6176,7 @@
         <v>69</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D55" s="29" t="s">
         <v>2</v>
@@ -6181,7 +6188,7 @@
         <v>91</v>
       </c>
       <c r="G55" s="33" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -6192,7 +6199,7 @@
         <v>69</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D56" s="29" t="s">
         <v>2</v>
@@ -6204,7 +6211,7 @@
         <v>91</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -6215,7 +6222,7 @@
         <v>69</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D57" s="29" t="s">
         <v>2</v>
@@ -6227,7 +6234,7 @@
         <v>91</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -6238,7 +6245,7 @@
         <v>69</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D58" s="29" t="s">
         <v>2</v>
@@ -6250,7 +6257,7 @@
         <v>91</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -6261,7 +6268,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D59" s="29" t="s">
         <v>2</v>
@@ -6273,7 +6280,7 @@
         <v>91</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -6284,7 +6291,7 @@
         <v>69</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D60" s="29" t="s">
         <v>2</v>
@@ -6296,7 +6303,7 @@
         <v>91</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -6307,7 +6314,7 @@
         <v>69</v>
       </c>
       <c r="C61" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D61" s="29" t="s">
         <v>2</v>
@@ -6319,7 +6326,7 @@
         <v>91</v>
       </c>
       <c r="G61" s="33" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -6330,7 +6337,7 @@
         <v>69</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D62" s="29" t="s">
         <v>2</v>
@@ -6342,7 +6349,7 @@
         <v>91</v>
       </c>
       <c r="G62" s="33" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -6353,7 +6360,7 @@
         <v>69</v>
       </c>
       <c r="C63" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D63" s="29" t="s">
         <v>2</v>
@@ -6365,7 +6372,7 @@
         <v>91</v>
       </c>
       <c r="G63" s="33" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -6376,7 +6383,7 @@
         <v>69</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D64" s="29" t="s">
         <v>2</v>
@@ -6388,7 +6395,7 @@
         <v>91</v>
       </c>
       <c r="G64" s="33" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -6399,7 +6406,7 @@
         <v>69</v>
       </c>
       <c r="C65" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D65" s="29" t="s">
         <v>2</v>
@@ -6411,18 +6418,18 @@
         <v>91</v>
       </c>
       <c r="G65" s="33" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="29" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="B66" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D66" s="29" t="s">
         <v>2</v>
@@ -6434,18 +6441,18 @@
         <v>91</v>
       </c>
       <c r="G66" s="33" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="29" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B67" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D67" s="29" t="s">
         <v>2</v>
@@ -6457,18 +6464,18 @@
         <v>91</v>
       </c>
       <c r="G67" s="32" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="29" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B68" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C68" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D68" s="29" t="s">
         <v>2</v>
@@ -6480,18 +6487,18 @@
         <v>91</v>
       </c>
       <c r="G68" s="32" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="29" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B69" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C69" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D69" s="29" t="s">
         <v>2</v>
@@ -6503,18 +6510,18 @@
         <v>91</v>
       </c>
       <c r="G69" s="72" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="29" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="B70" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D70" s="29" t="s">
         <v>2</v>
@@ -6526,18 +6533,18 @@
         <v>91</v>
       </c>
       <c r="G70" s="32" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="29" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="B71" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C71" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D71" s="29" t="s">
         <v>2</v>
@@ -6549,18 +6556,18 @@
         <v>91</v>
       </c>
       <c r="G71" s="32" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="29" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B72" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C72" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D72" s="29" t="s">
         <v>2</v>
@@ -6572,18 +6579,18 @@
         <v>91</v>
       </c>
       <c r="G72" s="32" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="29" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B73" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C73" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D73" s="29" t="s">
         <v>2</v>
@@ -6595,18 +6602,18 @@
         <v>91</v>
       </c>
       <c r="G73" s="32" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="29" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B74" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C74" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>2</v>
@@ -6618,18 +6625,18 @@
         <v>91</v>
       </c>
       <c r="G74" s="32" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="29" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="B75" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C75" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D75" s="29" t="s">
         <v>2</v>
@@ -6641,18 +6648,18 @@
         <v>91</v>
       </c>
       <c r="G75" s="32" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="29" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="B76" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C76" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D76" s="29" t="s">
         <v>2</v>
@@ -6664,7 +6671,7 @@
         <v>91</v>
       </c>
       <c r="G76" s="32" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -6701,7 +6708,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>68</v>
@@ -6713,13 +6720,13 @@
         <v>10</v>
       </c>
       <c r="F1" s="56" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H1" s="56" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="285">
@@ -6727,25 +6734,25 @@
         <v>4</v>
       </c>
       <c r="B2" s="57" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="D2" s="82" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="E2" s="57" t="s">
         <v>117</v>
       </c>
       <c r="F2" s="74" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="G2" s="65" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="75">
@@ -6753,25 +6760,25 @@
         <v>9</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>125</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="P3" s="73"/>
     </row>
@@ -6934,7 +6941,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7067,7 +7074,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>2</v>
@@ -7079,13 +7086,13 @@
         <v>69</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>35</v>
@@ -7161,7 +7168,7 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A2" s="18" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>57</v>
@@ -7189,12 +7196,12 @@
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="13" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A3" s="18" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="21" t="s">
@@ -7220,12 +7227,12 @@
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="33" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A4" s="18" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="21" t="s">
@@ -7251,12 +7258,12 @@
       </c>
       <c r="J4" s="23"/>
       <c r="K4" s="33" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A5" s="18" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>57</v>
@@ -7284,12 +7291,12 @@
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="33" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A6" s="18" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="21" t="s">
@@ -7315,12 +7322,12 @@
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="33" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A7" s="18" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="21" t="s">
@@ -7346,12 +7353,12 @@
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="33" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A8" s="18" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="21" t="s">
@@ -7377,12 +7384,12 @@
       </c>
       <c r="J8" s="23"/>
       <c r="K8" s="33" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A9" s="18" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="21" t="s">
@@ -7408,12 +7415,12 @@
       </c>
       <c r="J9" s="23"/>
       <c r="K9" s="33" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A10" s="18" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="21" t="s">
@@ -7439,12 +7446,12 @@
       </c>
       <c r="J10" s="23"/>
       <c r="K10" s="33" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" ht="60">
       <c r="A11" s="18" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="21" t="s">
@@ -7470,12 +7477,12 @@
       </c>
       <c r="J11" s="23"/>
       <c r="K11" s="33" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="60">
       <c r="A12" s="18" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="21" t="s">
@@ -7501,12 +7508,12 @@
       </c>
       <c r="J12" s="23"/>
       <c r="K12" s="33" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60">
       <c r="A13" s="18" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="21" t="s">
@@ -7532,12 +7539,12 @@
       </c>
       <c r="J13" s="23"/>
       <c r="K13" s="33" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="18" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="21" t="s">
@@ -7566,7 +7573,7 @@
     </row>
     <row r="15" spans="1:11" ht="60">
       <c r="A15" s="18" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="21" t="s">
@@ -7595,7 +7602,7 @@
     </row>
     <row r="16" spans="1:11" ht="60">
       <c r="A16" s="18" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="21" t="s">
@@ -7624,7 +7631,7 @@
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="18" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="21" t="s">
@@ -7653,7 +7660,7 @@
     </row>
     <row r="18" spans="1:11" ht="60">
       <c r="A18" s="18" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>57</v>
@@ -7684,7 +7691,7 @@
     </row>
     <row r="19" spans="1:11" ht="60">
       <c r="A19" s="18" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="21" t="s">
@@ -7713,7 +7720,7 @@
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" s="18" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="21" t="s">
@@ -7739,12 +7746,12 @@
       </c>
       <c r="J20" s="23"/>
       <c r="K20" s="33" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="60">
       <c r="A21" s="18" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="21" t="s">
@@ -7770,12 +7777,12 @@
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="33" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60">
       <c r="A22" s="18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="21" t="s">
@@ -7801,12 +7808,12 @@
       </c>
       <c r="J22" s="23"/>
       <c r="K22" s="33" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60">
       <c r="A23" s="18" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="21" t="s">
@@ -7832,12 +7839,12 @@
       </c>
       <c r="J23" s="23"/>
       <c r="K23" s="33" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60">
       <c r="A24" s="18" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B24" s="18"/>
       <c r="C24" s="21" t="s">
@@ -7863,12 +7870,12 @@
       </c>
       <c r="J24" s="23"/>
       <c r="K24" s="33" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60">
       <c r="A25" s="18" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="21" t="s">
@@ -7894,12 +7901,12 @@
       </c>
       <c r="J25" s="23"/>
       <c r="K25" s="33" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60">
       <c r="A26" s="18" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="21" t="s">
@@ -7925,12 +7932,12 @@
       </c>
       <c r="J26" s="23"/>
       <c r="K26" s="33" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60">
       <c r="A27" s="18" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="21" t="s">
@@ -7956,12 +7963,12 @@
       </c>
       <c r="J27" s="23"/>
       <c r="K27" s="33" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" s="18" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="21" t="s">
@@ -7987,12 +7994,12 @@
       </c>
       <c r="J28" s="23"/>
       <c r="K28" s="33" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60">
       <c r="A29" s="18" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="21" t="s">
@@ -8018,12 +8025,12 @@
       </c>
       <c r="J29" s="23"/>
       <c r="K29" s="33" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60">
       <c r="A30" s="18" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="21" t="s">
@@ -8049,12 +8056,12 @@
       </c>
       <c r="J30" s="23"/>
       <c r="K30" s="33" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60">
       <c r="A31" s="18" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="21" t="s">
@@ -8080,12 +8087,12 @@
       </c>
       <c r="J31" s="23"/>
       <c r="K31" s="33" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="60">
       <c r="A32" s="18" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="21" t="s">
@@ -8114,7 +8121,7 @@
     </row>
     <row r="33" spans="1:11" ht="60">
       <c r="A33" s="18" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="21" t="s">
@@ -8143,7 +8150,7 @@
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" s="18" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="21" t="s">
@@ -8172,7 +8179,7 @@
     </row>
     <row r="35" spans="1:11" ht="60">
       <c r="A35" s="18" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>57</v>
@@ -8203,7 +8210,7 @@
     </row>
     <row r="36" spans="1:11" ht="60">
       <c r="A36" s="18" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="21" t="s">
@@ -8232,7 +8239,7 @@
     </row>
     <row r="37" spans="1:11" ht="60">
       <c r="A37" s="18" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="21" t="s">
@@ -8261,7 +8268,7 @@
     </row>
     <row r="38" spans="1:11" ht="60">
       <c r="A38" s="18" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="21" t="s">
@@ -8290,7 +8297,7 @@
     </row>
     <row r="39" spans="1:11" ht="60">
       <c r="A39" s="18" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="21" t="s">
@@ -8300,7 +8307,7 @@
         <v>89</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>48</v>
@@ -8319,16 +8326,16 @@
     </row>
     <row r="40" spans="1:11" ht="60">
       <c r="A40" s="18" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>4</v>
@@ -8347,7 +8354,7 @@
       </c>
       <c r="J40" s="23"/>
       <c r="K40" s="71" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -8395,13 +8402,13 @@
         <v>14</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8410,10 +8417,10 @@
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="75" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D2" s="76" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E2" s="58" t="s">
         <v>4</v>
@@ -8427,7 +8434,7 @@
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="75" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="D3" s="76" t="s">
         <v>68</v>
@@ -8444,10 +8451,10 @@
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="75" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D4" s="76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E4" s="58" t="s">
         <v>4</v>
@@ -8461,10 +8468,10 @@
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="75" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="E5" s="58" t="s">
         <v>4</v>
@@ -8478,10 +8485,10 @@
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="75" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E6" s="58" t="s">
         <v>4</v>
@@ -8495,10 +8502,10 @@
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="75" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D7" s="76" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="E7" s="58" t="s">
         <v>4</v>
@@ -8512,10 +8519,10 @@
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="75" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="D8" s="76" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>4</v>
@@ -8531,10 +8538,10 @@
         <v>57</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D9" s="76" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="E9" s="58" t="s">
         <v>4</v>
@@ -8597,40 +8604,40 @@
         <v>13</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>121</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30">
       <c r="A2" s="85" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D2" s="64" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>9</v>
@@ -8639,32 +8646,32 @@
       <c r="G2" s="27"/>
       <c r="H2" s="29"/>
       <c r="I2" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" ht="45">
       <c r="A3" s="85" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="27" t="s">
+        <v>554</v>
+      </c>
+      <c r="D3" s="64" t="s">
         <v>559</v>
-      </c>
-      <c r="D3" s="64" t="s">
-        <v>564</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>9</v>
@@ -8673,32 +8680,32 @@
       <c r="G3" s="27"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:14" ht="45">
       <c r="A4" s="85" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>9</v>
@@ -8707,32 +8714,32 @@
       <c r="G4" s="27"/>
       <c r="H4" s="29"/>
       <c r="I4" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K4" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M4" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:14" ht="60">
       <c r="A5" s="86" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B5" s="86"/>
       <c r="C5" s="87" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D5" s="88" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="E5" s="86" t="s">
         <v>9</v>
@@ -8740,37 +8747,37 @@
       <c r="F5" s="87"/>
       <c r="G5" s="87"/>
       <c r="H5" s="86" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I5" s="86" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J5" s="86" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K5" s="86" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L5" s="86" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M5" s="86" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="N5" s="87" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45">
       <c r="A6" s="85" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="23" t="s">
         <v>120</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>9</v>
@@ -8781,34 +8788,34 @@
         <v>122</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30">
       <c r="A7" s="85" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>9</v>
@@ -8817,32 +8824,32 @@
       <c r="G7" s="27"/>
       <c r="H7" s="29"/>
       <c r="I7" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14" ht="30">
       <c r="A8" s="85" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>9</v>
@@ -8851,358 +8858,358 @@
       <c r="G8" s="27"/>
       <c r="H8" s="29"/>
       <c r="I8" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K8" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M8" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:14" ht="30">
       <c r="A9" s="85" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G9" s="27"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K9" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L9" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M9" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" ht="45">
       <c r="A10" s="85" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G10" s="27"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K10" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N10" s="23"/>
     </row>
     <row r="11" spans="1:14" ht="45">
       <c r="A11" s="85" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="B11" s="29"/>
       <c r="C11" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G11" s="27"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K11" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L11" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M11" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" ht="60">
       <c r="A12" s="85" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G12" s="27"/>
       <c r="H12" s="29" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I12" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K12" s="29"/>
       <c r="L12" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M12" s="29"/>
       <c r="N12" s="23" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45">
       <c r="A13" s="85" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="23" t="s">
         <v>120</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G13" s="27"/>
       <c r="H13" s="29" t="s">
         <v>122</v>
       </c>
       <c r="I13" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K13" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L13" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M13" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N13" s="23" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30">
       <c r="A14" s="85" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="B14" s="29"/>
       <c r="C14" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G14" s="27"/>
       <c r="H14" s="29"/>
       <c r="I14" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K14" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M14" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" ht="30">
       <c r="A15" s="85" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B15" s="29"/>
       <c r="C15" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G15" s="27"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J15" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K15" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" ht="105">
       <c r="A16" s="85" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B16" s="29" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="E16" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="29" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K16" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M16" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N16" s="23" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="105">
       <c r="A17" s="85" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="27" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="E17" s="29" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="G17" s="27"/>
       <c r="H17" s="29" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J17" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K17" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="N17" s="23" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -9251,69 +9258,69 @@
         <v>15</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="H1" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="I1" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="J1" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="K1" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="36" t="s">
         <v>223</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="N1" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="4" customFormat="1">
       <c r="A2" s="37" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="G2" s="38">
         <v>300389093</v>
@@ -9328,7 +9335,7 @@
         <v>3</v>
       </c>
       <c r="K2" s="40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L2" s="41">
         <v>3</v>
@@ -9354,22 +9361,22 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="37" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="G3" s="38">
         <v>300389094</v>
@@ -9384,7 +9391,7 @@
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L3" s="41">
         <v>2</v>
@@ -9410,22 +9417,22 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="37" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>242</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G4" s="38">
         <v>300389095</v>
@@ -9440,7 +9447,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L4" s="41">
         <v>1</v>
@@ -9466,22 +9473,22 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="37" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>245</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G5" s="38">
         <v>300389095</v>
@@ -9584,13 +9591,13 @@
         <v>6</v>
       </c>
       <c r="F1" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45">
@@ -9601,19 +9608,19 @@
         <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D2" s="55" t="s">
         <v>149</v>
       </c>
       <c r="E2" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="H2" s="2">
         <v>0</v>
@@ -9627,19 +9634,19 @@
         <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D3" s="55" t="s">
         <v>150</v>
       </c>
       <c r="E3" s="54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -9653,13 +9660,13 @@
         <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D4" s="67" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E4" s="54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -9708,7 +9715,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9719,13 +9726,13 @@
         <v>57</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E2" s="54" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -9734,13 +9741,13 @@
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="32" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E3" s="54" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
@@ -9751,13 +9758,13 @@
         <v>57</v>
       </c>
       <c r="C4" s="78" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E4" s="79" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -9768,13 +9775,13 @@
         <v>57</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
@@ -9785,13 +9792,13 @@
         <v>57</v>
       </c>
       <c r="C6" s="78" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E6" s="79" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
@@ -9802,13 +9809,13 @@
         <v>57</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -9822,22 +9829,23 @@
   <sheetPr codeName="Sheet9">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="15" t="s">
         <v>78</v>
       </c>
@@ -9847,42 +9855,53 @@
       <c r="C1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="47" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="47" t="s">
+        <v>584</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>528</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60">
+      <c r="A3" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="47" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="47" t="s">
-        <v>369</v>
-      </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="48" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>533</v>
-      </c>
-      <c r="E3" s="47" t="s">
+      <c r="D3" s="48" t="s">
+        <v>585</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>528</v>
+      </c>
+      <c r="F3" s="47" t="s">
         <v>65</v>
       </c>
     </row>
@@ -9897,22 +9916,21 @@
   <sheetPr codeName="Sheet10">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:8">
       <c r="A1" s="15" t="s">
         <v>78</v>
       </c>
@@ -9929,22 +9947,16 @@
         <v>8</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="60">
+    <row r="2" spans="1:8" ht="30">
       <c r="A2" s="30" t="s">
         <v>79</v>
       </c>
@@ -9952,60 +9964,22 @@
         <v>57</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>277</v>
+        <v>580</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>257</v>
+        <v>581</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>16</v>
       </c>
       <c r="G2" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="49" t="s">
-        <v>256</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="60">
-      <c r="A3" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>258</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="49" t="s">
-        <v>256</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>149</v>
+        <v>65</v>
+      </c>
+      <c r="H2" s="78" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change user mail to code
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="258360" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="261150" yWindow="0" windowWidth="16980" windowHeight="7020" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AccountSetupRegression" sheetId="37" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="381">
   <si>
     <t>Accept</t>
   </si>
@@ -242,30 +242,6 @@
     <t>caseId</t>
   </si>
   <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>T8</t>
-  </si>
-  <si>
     <t>guest
 new-user
 new-shipping
@@ -501,24 +477,6 @@
   </si>
   <si>
     <t>overview</t>
-  </si>
-  <si>
-    <t>id
-title
-price
-overview
-feature
-stock availability
-add to cart button</t>
-  </si>
-  <si>
-    <t>feature</t>
-  </si>
-  <si>
-    <t>stock availability</t>
-  </si>
-  <si>
-    <t>add to cart button</t>
   </si>
   <si>
     <t>Guest, verify the PDP basics id</t>
@@ -713,52 +671,10 @@
     <t>Provide a valid promotion code.</t>
   </si>
   <si>
-    <t>loggedin
-Verify unit Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loggedin
-Verify subtotal
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loggedin
-Verify discount
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loggedin
-Verify Promotion
-remove Promotion
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loggedin
-Verify Promotion
-</t>
-  </si>
-  <si>
-    <t>loggedin
-Verify clubDiscount</t>
-  </si>
-  <si>
-    <t>loggedin
-Verify total</t>
-  </si>
-  <si>
     <t>$0.00</t>
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>loggedin
-Verify unit Price
-Verify subtotal
-Verify discount
-Verify Promotion
-Verify clubDiscount
-Verify total</t>
   </si>
   <si>
     <t>ValidationMSG</t>
@@ -1164,6 +1080,199 @@
   </si>
   <si>
     <t>U-24</t>
+  </si>
+  <si>
+    <t>U-25</t>
+  </si>
+  <si>
+    <t>Loggedin
+Verify unit Price
+Verify subtotal
+Verify discount
+Verify Promotion
+Verify clubDiscount
+Verify total</t>
+  </si>
+  <si>
+    <t>Loggedin
+Verify unit Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggedin
+Verify subtotal
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggedin
+Verify discount
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggedin
+Verify Promotion
+remove Promotion
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggedin
+Verify Promotion
+</t>
+  </si>
+  <si>
+    <t>Loggedin
+Verify clubDiscount</t>
+  </si>
+  <si>
+    <t>Loggedin
+Verify total</t>
+  </si>
+  <si>
+    <t>Loggedin, verify the PDP basics id</t>
+  </si>
+  <si>
+    <t>Loggedin, verify the PDP basics title</t>
+  </si>
+  <si>
+    <t>Loggedin, verify the PDP basics price</t>
+  </si>
+  <si>
+    <t>Loggedin, verify the PDP basics overview</t>
+  </si>
+  <si>
+    <t>Loggedin, verify the PDP basics features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggedin, verify the PDP basics availability </t>
+  </si>
+  <si>
+    <t>Loggedin, verify the PDP basics add to cart button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loggedin, verify the PDP basics </t>
+  </si>
+  <si>
+    <t>Guest
+id</t>
+  </si>
+  <si>
+    <t>Guest
+title</t>
+  </si>
+  <si>
+    <t>Guest
+price</t>
+  </si>
+  <si>
+    <t>Guest
+overview</t>
+  </si>
+  <si>
+    <t>Guest
+feature</t>
+  </si>
+  <si>
+    <t>Guest
+stock availability</t>
+  </si>
+  <si>
+    <t>Guest
+add to cart button</t>
+  </si>
+  <si>
+    <t>Guest
+id
+title
+price
+overview
+feature
+stock availability
+add to cart button</t>
+  </si>
+  <si>
+    <t>Loggedin
+id</t>
+  </si>
+  <si>
+    <t>Loggedin
+title</t>
+  </si>
+  <si>
+    <t>Loggedin
+price</t>
+  </si>
+  <si>
+    <t>Loggedin
+overview</t>
+  </si>
+  <si>
+    <t>Loggedin
+feature</t>
+  </si>
+  <si>
+    <t>Loggedin
+stock availability</t>
+  </si>
+  <si>
+    <t>Loggedin
+add to cart button</t>
+  </si>
+  <si>
+    <t>Loggedin
+id
+title
+price
+overview
+feature
+stock availability
+add to cart button</t>
+  </si>
+  <si>
+    <t>PDP-01</t>
+  </si>
+  <si>
+    <t>PDP-02</t>
+  </si>
+  <si>
+    <t>PDP-03</t>
+  </si>
+  <si>
+    <t>PDP-04</t>
+  </si>
+  <si>
+    <t>PDP-05</t>
+  </si>
+  <si>
+    <t>PDP-06</t>
+  </si>
+  <si>
+    <t>PDP-07</t>
+  </si>
+  <si>
+    <t>PDP-08</t>
+  </si>
+  <si>
+    <t>PDP-09</t>
+  </si>
+  <si>
+    <t>PDP-10</t>
+  </si>
+  <si>
+    <t>PDP-11</t>
+  </si>
+  <si>
+    <t>PDP-12</t>
+  </si>
+  <si>
+    <t>PDP-13</t>
+  </si>
+  <si>
+    <t>PDP-14</t>
+  </si>
+  <si>
+    <t>PDP-15</t>
+  </si>
+  <si>
+    <t>PDP-16</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1498,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1528,9 +1637,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1583,6 +1689,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1934,22 +2048,22 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="H39" sqref="A1:XFD1048576"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="53"/>
-    <col min="3" max="3" width="9.5703125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.85546875" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5703125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.5703125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="2" width="9.140625" style="52"/>
+    <col min="3" max="3" width="9.5703125" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.85546875" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5703125" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="59" customFormat="1">
+    <row r="1" spans="1:8" s="58" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>69</v>
       </c>
@@ -1975,19 +2089,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="61" customFormat="1">
+    <row r="2" spans="1:8" s="60" customFormat="1">
       <c r="A2" s="21" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>60</v>
@@ -1995,23 +2109,23 @@
       <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="61" customFormat="1">
+      <c r="H2" s="17" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="60" customFormat="1">
       <c r="A3" s="21" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>60</v>
@@ -2019,23 +2133,23 @@
       <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="61" customFormat="1">
+      <c r="H3" s="17" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="60" customFormat="1">
       <c r="A4" s="21" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>60</v>
@@ -2043,23 +2157,23 @@
       <c r="G4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="61" customFormat="1">
+      <c r="H4" s="17" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="60" customFormat="1">
       <c r="A5" s="21" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>60</v>
@@ -2067,23 +2181,23 @@
       <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="61" customFormat="1">
+      <c r="H5" s="17" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="60" customFormat="1">
       <c r="A6" s="21" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>60</v>
@@ -2091,23 +2205,23 @@
       <c r="G6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="61" customFormat="1">
+      <c r="H6" s="17" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="60" customFormat="1">
       <c r="A7" s="21" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>60</v>
@@ -2115,20 +2229,20 @@
       <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="19" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="61" customFormat="1">
+      <c r="H7" s="17" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="60" customFormat="1">
       <c r="A8" s="21" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>13</v>
@@ -2139,20 +2253,20 @@
       <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="61" customFormat="1">
+      <c r="H8" s="17" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="60" customFormat="1">
       <c r="A9" s="21" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>13</v>
@@ -2163,20 +2277,20 @@
       <c r="G9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="61" customFormat="1">
+      <c r="H9" s="17" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="60" customFormat="1">
       <c r="A10" s="21" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>13</v>
@@ -2187,20 +2301,20 @@
       <c r="G10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>262</v>
+      <c r="H10" s="17" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>13</v>
@@ -2211,20 +2325,20 @@
       <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>263</v>
+      <c r="H11" s="17" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="21" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B12" s="21"/>
       <c r="C12" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>13</v>
@@ -2235,13 +2349,13 @@
       <c r="G12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="19" t="s">
-        <v>264</v>
+      <c r="H12" s="17" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="21" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>52</v>
@@ -2250,7 +2364,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>13</v>
@@ -2261,20 +2375,20 @@
       <c r="G13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>285</v>
+      <c r="H13" s="17" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="21" t="s">
-        <v>288</v>
+        <v>268</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>13</v>
@@ -2285,20 +2399,20 @@
       <c r="G14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>299</v>
+      <c r="H14" s="17" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="21" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>13</v>
@@ -2309,20 +2423,20 @@
       <c r="G15" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>300</v>
+      <c r="H15" s="17" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="21" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>13</v>
@@ -2333,13 +2447,13 @@
       <c r="G16" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="19" t="s">
-        <v>286</v>
+      <c r="H16" s="17" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="21" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>52</v>
@@ -2348,7 +2462,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>13</v>
@@ -2359,20 +2473,20 @@
       <c r="G17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H17" s="19" t="s">
-        <v>301</v>
+      <c r="H17" s="17" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="21" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>13</v>
@@ -2383,20 +2497,20 @@
       <c r="G18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>302</v>
+      <c r="H18" s="17" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="21" t="s">
-        <v>293</v>
+        <v>273</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>13</v>
@@ -2407,20 +2521,20 @@
       <c r="G19" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="19" t="s">
-        <v>303</v>
+      <c r="H19" s="17" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="21" t="s">
-        <v>294</v>
+        <v>274</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>13</v>
@@ -2431,20 +2545,20 @@
       <c r="G20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>304</v>
+      <c r="H20" s="17" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="21" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>13</v>
@@ -2455,13 +2569,13 @@
       <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="19" t="s">
-        <v>305</v>
+      <c r="H21" s="17" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="21" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>52</v>
@@ -2470,7 +2584,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>13</v>
@@ -2481,20 +2595,20 @@
       <c r="G22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="19" t="s">
-        <v>306</v>
+      <c r="H22" s="17" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="21" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>13</v>
@@ -2505,20 +2619,20 @@
       <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>307</v>
+      <c r="H23" s="17" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="21" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="41" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E24" s="23" t="s">
         <v>13</v>
@@ -2529,8 +2643,8 @@
       <c r="G24" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H24" s="19" t="s">
-        <v>308</v>
+      <c r="H24" s="17" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -2544,20 +2658,20 @@
   <sheetPr codeName="Sheet19">
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="53"/>
-    <col min="3" max="3" width="10.140625" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.85546875" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="9.42578125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.5703125" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="2" width="9.140625" style="52"/>
+    <col min="3" max="3" width="10.140625" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.85546875" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="9.42578125" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.5703125" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2568,7 +2682,7 @@
         <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>35</v>
@@ -2585,13 +2699,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="17" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>0</v>
@@ -2600,21 +2714,21 @@
         <v>1</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="17" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>0</v>
@@ -2623,21 +2737,21 @@
         <v>1</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="17" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>0</v>
@@ -2646,21 +2760,21 @@
         <v>1</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="17" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>0</v>
@@ -2669,21 +2783,21 @@
         <v>1</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="17" t="s">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>0</v>
@@ -2692,21 +2806,21 @@
         <v>1</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="17" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>0</v>
@@ -2715,21 +2829,21 @@
         <v>1</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="17" t="s">
-        <v>334</v>
+        <v>314</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>0</v>
@@ -2738,21 +2852,21 @@
         <v>1</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="17" t="s">
-        <v>335</v>
+        <v>315</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>0</v>
@@ -2761,21 +2875,21 @@
         <v>1</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>260</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="17" t="s">
-        <v>336</v>
+        <v>316</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>0</v>
@@ -2784,21 +2898,21 @@
         <v>1</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="17" t="s">
-        <v>337</v>
+        <v>317</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>0</v>
@@ -2807,21 +2921,21 @@
         <v>1</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>262</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="17" t="s">
-        <v>338</v>
+        <v>318</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>0</v>
@@ -2830,21 +2944,21 @@
         <v>1</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>263</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="17" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>0</v>
@@ -2853,21 +2967,21 @@
         <v>1</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="17" t="s">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>0</v>
@@ -2876,21 +2990,21 @@
         <v>1</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>285</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="17" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>0</v>
@@ -2899,21 +3013,21 @@
         <v>1</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="17" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>0</v>
@@ -2922,21 +3036,21 @@
         <v>1</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="17" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>0</v>
@@ -2945,21 +3059,21 @@
         <v>1</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="17" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>0</v>
@@ -2968,21 +3082,21 @@
         <v>1</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="17" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>0</v>
@@ -2991,21 +3105,21 @@
         <v>1</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="17" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>0</v>
@@ -3014,21 +3128,21 @@
         <v>1</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="17" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>0</v>
@@ -3037,21 +3151,21 @@
         <v>1</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="17" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>0</v>
@@ -3060,21 +3174,21 @@
         <v>1</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="17" t="s">
-        <v>349</v>
+        <v>329</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>0</v>
@@ -3083,21 +3197,21 @@
         <v>1</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="17" t="s">
-        <v>350</v>
+        <v>330</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>0</v>
@@ -3106,21 +3220,21 @@
         <v>1</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="17" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>0</v>
@@ -3129,10 +3243,33 @@
         <v>1</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>308</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3151,7 +3288,7 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3169,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>61</v>
@@ -3181,13 +3318,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="75">
@@ -3195,25 +3332,25 @@
         <v>2</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="75">
@@ -3221,56 +3358,56 @@
         <v>6</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="P3" s="32"/>
     </row>
     <row r="4" spans="1:16" ht="180">
       <c r="A4" s="34" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="B4" s="34">
         <v>7783624</v>
       </c>
-      <c r="C4" s="49" t="s">
-        <v>324</v>
-      </c>
-      <c r="D4" s="66" t="s">
-        <v>325</v>
+      <c r="C4" s="48" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>305</v>
       </c>
       <c r="E4" s="34">
         <v>1</v>
       </c>
-      <c r="F4" s="49" t="s">
-        <v>326</v>
+      <c r="F4" s="48" t="s">
+        <v>306</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="H4" s="49" t="s">
-        <v>327</v>
+        <v>300</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="D5" s="65"/>
+      <c r="D5" s="64"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3324,7 +3461,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>23</v>
@@ -3558,7 +3695,7 @@
         <v>58</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>57</v>
@@ -3569,7 +3706,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>0</v>
@@ -3581,13 +3718,13 @@
         <v>62</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>31</v>
@@ -3610,7 +3747,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="A1:K20"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3623,7 +3760,7 @@
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6" style="67" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1">
@@ -3663,13 +3800,13 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="60">
       <c r="A2" s="8" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>56</v>
@@ -3678,10 +3815,10 @@
         <v>6</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G2" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H2" s="46" t="s">
         <v>60</v>
@@ -3690,19 +3827,17 @@
         <v>60</v>
       </c>
       <c r="J2" s="46"/>
-      <c r="K2" s="47" t="s">
-        <v>254</v>
+      <c r="K2" s="46" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="60">
       <c r="A3" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="B3" s="8"/>
       <c r="C3" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>56</v>
@@ -3711,10 +3846,10 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H3" s="46" t="s">
         <v>60</v>
@@ -3723,17 +3858,15 @@
         <v>60</v>
       </c>
       <c r="J3" s="46"/>
-      <c r="K3" s="47" t="s">
-        <v>255</v>
+      <c r="K3" s="46" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="60">
       <c r="A4" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
@@ -3744,10 +3877,10 @@
         <v>6</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="G4" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H4" s="46" t="s">
         <v>60</v>
@@ -3756,31 +3889,31 @@
         <v>60</v>
       </c>
       <c r="J4" s="46"/>
-      <c r="K4" s="48" t="s">
-        <v>264</v>
+      <c r="K4" s="46" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="60">
       <c r="A5" s="8" t="s">
-        <v>274</v>
+        <v>254</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G5" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H5" s="46" t="s">
         <v>60</v>
@@ -3793,25 +3926,25 @@
     </row>
     <row r="6" spans="1:11" ht="60">
       <c r="A6" s="8" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G6" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H6" s="46" t="s">
         <v>60</v>
@@ -3821,30 +3954,28 @@
       </c>
       <c r="J6" s="46"/>
       <c r="K6" s="47" t="s">
-        <v>256</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="60">
       <c r="A7" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H7" s="46" t="s">
         <v>60</v>
@@ -3853,31 +3984,29 @@
         <v>60</v>
       </c>
       <c r="J7" s="46"/>
-      <c r="K7" s="47" t="s">
-        <v>257</v>
+      <c r="K7" s="46" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60">
       <c r="A8" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G8" s="45" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="H8" s="46" t="s">
         <v>60</v>
@@ -3886,19 +4015,17 @@
         <v>60</v>
       </c>
       <c r="J8" s="46"/>
-      <c r="K8" s="47" t="s">
-        <v>258</v>
+      <c r="K8" s="46" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60">
       <c r="A9" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>56</v>
@@ -3907,7 +4034,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G9" s="45" t="s">
         <v>13</v>
@@ -3919,19 +4046,17 @@
         <v>60</v>
       </c>
       <c r="J9" s="46"/>
-      <c r="K9" s="47" t="s">
-        <v>259</v>
+      <c r="K9" s="46" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="60">
       <c r="A10" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>56</v>
@@ -3940,7 +4065,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G10" s="45" t="s">
         <v>13</v>
@@ -3952,17 +4077,15 @@
         <v>60</v>
       </c>
       <c r="J10" s="46"/>
-      <c r="K10" s="47" t="s">
-        <v>260</v>
+      <c r="K10" s="46" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60">
       <c r="A11" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
         <v>18</v>
       </c>
@@ -3973,7 +4096,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G11" s="45" t="s">
         <v>13</v>
@@ -3985,28 +4108,26 @@
         <v>60</v>
       </c>
       <c r="J11" s="46"/>
-      <c r="K11" s="47" t="s">
-        <v>261</v>
+      <c r="K11" s="46" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="60">
       <c r="A12" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G12" s="45" t="s">
         <v>13</v>
@@ -4022,22 +4143,20 @@
     </row>
     <row r="13" spans="1:11" ht="60">
       <c r="A13" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>262</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G13" s="45" t="s">
         <v>13</v>
@@ -4053,22 +4172,20 @@
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G14" s="45" t="s">
         <v>13</v>
@@ -4084,22 +4201,20 @@
     </row>
     <row r="15" spans="1:11" ht="60">
       <c r="A15" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>264</v>
+      </c>
+      <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G15" s="45" t="s">
         <v>13</v>
@@ -4115,22 +4230,20 @@
     </row>
     <row r="16" spans="1:11" ht="60">
       <c r="A16" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G16" s="45" t="s">
         <v>13</v>
@@ -4146,22 +4259,20 @@
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="B17" s="8"/>
       <c r="C17" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G17" s="45" t="s">
         <v>13</v>
@@ -4177,22 +4288,20 @@
     </row>
     <row r="18" spans="1:11" ht="60">
       <c r="A18" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G18" s="45" t="s">
         <v>13</v>
@@ -4208,22 +4317,20 @@
     </row>
     <row r="19" spans="1:11" ht="60">
       <c r="A19" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>52</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G19" s="45" t="s">
         <v>13</v>
@@ -4239,22 +4346,22 @@
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="G20" s="45" t="s">
         <v>13</v>
@@ -4266,8 +4373,8 @@
         <v>60</v>
       </c>
       <c r="J20" s="46"/>
-      <c r="K20" s="47" t="s">
-        <v>262</v>
+      <c r="K20" s="46" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4281,183 +4388,337 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="8" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:G9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="8" t="s">
-        <v>70</v>
+        <v>365</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="64" t="s">
+      <c r="C2" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>349</v>
+      </c>
+      <c r="E2" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="45"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="8" t="s">
-        <v>71</v>
+        <v>366</v>
       </c>
       <c r="B3" s="8"/>
-      <c r="C3" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="64" t="s">
+      <c r="C3" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>350</v>
+      </c>
+      <c r="E3" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="28"/>
       <c r="G3" s="45"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="8" t="s">
-        <v>72</v>
+        <v>367</v>
       </c>
       <c r="B4" s="8"/>
-      <c r="C4" s="62" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="64" t="s">
+      <c r="C4" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="62" t="s">
+        <v>351</v>
+      </c>
+      <c r="E4" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="45"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="8" t="s">
-        <v>73</v>
+        <v>368</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="62" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="64" t="s">
+      <c r="C5" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>352</v>
+      </c>
+      <c r="E5" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="28"/>
-      <c r="G5" s="45"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5" s="68"/>
+    </row>
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="8" t="s">
-        <v>74</v>
+        <v>369</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="62" t="s">
-        <v>160</v>
-      </c>
-      <c r="D6" s="63" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="64" t="s">
+      <c r="C6" s="61" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="28"/>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="68"/>
+    </row>
+    <row r="7" spans="1:7" ht="30">
       <c r="A7" s="8" t="s">
-        <v>75</v>
+        <v>370</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="62" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="63" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="64" t="s">
+      <c r="C7" s="61" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>354</v>
+      </c>
+      <c r="E7" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="28"/>
-      <c r="G7" s="45"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="68"/>
+    </row>
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="8" t="s">
-        <v>76</v>
+        <v>371</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>155</v>
-      </c>
-      <c r="E8" s="64" t="s">
+      <c r="C8" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="62" t="s">
+        <v>355</v>
+      </c>
+      <c r="E8" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="28"/>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:7" ht="105">
+      <c r="G8" s="68"/>
+    </row>
+    <row r="9" spans="1:7" ht="120">
       <c r="A9" s="8" t="s">
-        <v>77</v>
+        <v>372</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="63" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9" s="64" t="s">
+      <c r="C9" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>356</v>
+      </c>
+      <c r="E9" s="63" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="28"/>
-      <c r="G9" s="45"/>
+      <c r="G9" s="68"/>
+    </row>
+    <row r="10" spans="1:7" ht="30">
+      <c r="A10" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="61" t="s">
+        <v>341</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>357</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="G10" s="69"/>
+    </row>
+    <row r="11" spans="1:7" ht="30">
+      <c r="A11" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="61" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>358</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="G11" s="69"/>
+    </row>
+    <row r="12" spans="1:7" ht="30">
+      <c r="A12" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="61" t="s">
+        <v>343</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>359</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="G12" s="69"/>
+    </row>
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="61" t="s">
+        <v>344</v>
+      </c>
+      <c r="D13" s="62" t="s">
+        <v>360</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="G13" s="69"/>
+    </row>
+    <row r="14" spans="1:7" ht="30">
+      <c r="A14" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="61" t="s">
+        <v>345</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>361</v>
+      </c>
+      <c r="E14" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="G14" s="69"/>
+    </row>
+    <row r="15" spans="1:7" ht="30">
+      <c r="A15" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="61" t="s">
+        <v>346</v>
+      </c>
+      <c r="D15" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="G15" s="69"/>
+    </row>
+    <row r="16" spans="1:7" ht="30">
+      <c r="A16" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="61" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>363</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="G16" s="69"/>
+    </row>
+    <row r="17" spans="1:7" ht="120">
+      <c r="A17" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>348</v>
+      </c>
+      <c r="D17" s="62" t="s">
+        <v>364</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="G17" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4472,8 +4733,8 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:N17"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4483,7 +4744,7 @@
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="12"/>
-    <col min="6" max="6" width="30.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="12" customWidth="1"/>
@@ -4514,42 +4775,40 @@
         <v>9</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30">
       <c r="A2" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>52</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B2" s="49"/>
       <c r="C2" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>6</v>
@@ -4558,34 +4817,32 @@
       <c r="G2" s="15"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:14" ht="45">
       <c r="A3" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>52</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="B3" s="49"/>
       <c r="C3" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>6</v>
@@ -4594,34 +4851,32 @@
       <c r="G3" s="15"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:14" ht="45">
       <c r="A4" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>52</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="B4" s="49"/>
       <c r="C4" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>6</v>
@@ -4630,72 +4885,68 @@
       <c r="G4" s="15"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" ht="60">
-      <c r="A5" s="50" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="51" t="s">
+      <c r="A5" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>299</v>
+      </c>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49" t="s">
+        <v>300</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>301</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>302</v>
+      </c>
+      <c r="L5" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="D5" s="52" t="s">
-        <v>210</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>319</v>
-      </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50" t="s">
-        <v>320</v>
-      </c>
-      <c r="J5" s="50" t="s">
-        <v>321</v>
-      </c>
-      <c r="K5" s="50" t="s">
-        <v>322</v>
-      </c>
-      <c r="L5" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="M5" s="50" t="s">
-        <v>323</v>
-      </c>
-      <c r="N5" s="51" t="s">
-        <v>220</v>
+      <c r="M5" s="49" t="s">
+        <v>303</v>
+      </c>
+      <c r="N5" s="50" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45">
       <c r="A6" s="38" t="s">
-        <v>186</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>52</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B6" s="49"/>
       <c r="C6" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>6</v>
@@ -4703,39 +4954,37 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="17" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="30">
       <c r="A7" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>52</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="B7" s="49"/>
       <c r="C7" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>6</v>
@@ -4744,34 +4993,32 @@
       <c r="G7" s="15"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M7" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14" ht="30">
       <c r="A8" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="49"/>
+      <c r="C8" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="B8" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>200</v>
-      </c>
       <c r="D8" s="29" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>6</v>
@@ -4780,306 +5027,292 @@
       <c r="G8" s="15"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L8" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:14" ht="30">
       <c r="A9" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="B9" s="17"/>
       <c r="C9" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>212</v>
+        <v>334</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>286</v>
+      <c r="F9" s="66" t="s">
+        <v>323</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:14" ht="45">
       <c r="A10" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>213</v>
+        <v>335</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J10" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:14" ht="45">
       <c r="A11" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="B11" s="17"/>
       <c r="C11" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>214</v>
+        <v>336</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14" ht="60">
       <c r="A12" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>52</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>215</v>
+        <v>337</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>286</v>
+        <v>323</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="45">
       <c r="A13" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="B13" s="17"/>
       <c r="C13" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>216</v>
+        <v>338</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="17" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L13" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N13" s="11" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30">
       <c r="A14" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="B14" s="17"/>
       <c r="C14" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>217</v>
+        <v>339</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" ht="30">
       <c r="A15" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="B15" s="17"/>
       <c r="C15" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>218</v>
+        <v>340</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>286</v>
+        <v>323</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14" ht="105">
       <c r="A16" s="38" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>6</v>
@@ -5088,67 +5321,68 @@
       <c r="G16" s="15"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L16" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N16" s="11" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="105">
       <c r="A17" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>52</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="B17" s="17"/>
       <c r="C17" s="15" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>221</v>
+        <v>333</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="N17" s="11" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F9" r:id="rId1" display="cart0022@OSH-automation.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5160,47 +5394,47 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="A1:XFD1048576"/>
+      <selection activeCell="K1" sqref="K1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="53"/>
-    <col min="3" max="3" width="26.5703125" style="53" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" style="61" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" style="53" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="2" width="9.140625" style="52"/>
+    <col min="3" max="3" width="26.5703125" style="52" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="60" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.140625" style="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="59" customFormat="1">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:5" s="58" customFormat="1">
+      <c r="A1" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="58" t="s">
-        <v>231</v>
+      <c r="D1" s="57" t="s">
+        <v>211</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="61" customFormat="1">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="60" customFormat="1">
       <c r="A2" s="8" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>232</v>
+        <v>99</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>212</v>
       </c>
       <c r="E2" s="11">
         <v>12</v>
@@ -5208,16 +5442,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="E3" s="11">
         <v>12</v>
@@ -5225,16 +5459,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="E4" s="11">
         <v>12</v>
@@ -5254,19 +5488,19 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="A1:XFD1048576"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="54"/>
-    <col min="3" max="3" width="37.42578125" style="53" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71" style="53" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="2" width="9.140625" style="53"/>
+    <col min="3" max="3" width="37.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71" style="52" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="54" customFormat="1">
+    <row r="1" spans="1:5" s="53" customFormat="1">
       <c r="A1" s="24" t="s">
         <v>69</v>
       </c>
@@ -5280,107 +5514,107 @@
         <v>10</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="46" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>114</v>
+        <v>105</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>106</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="46" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>116</v>
+        <v>107</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>108</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
       <c r="A4" s="46" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="56" t="s">
-        <v>118</v>
+        <v>157</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>110</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="46" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>112</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="46" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="56" t="s">
-        <v>122</v>
+        <v>113</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>114</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45">
       <c r="A7" s="46" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>124</v>
+      <c r="C7" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>116</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5397,18 +5631,18 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="A1:XFD1048576"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" style="53" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="53" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="53" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="1" width="6.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="52" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="52" customWidth="1"/>
+    <col min="5" max="5" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="52" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5422,30 +5656,30 @@
         <v>11</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="21" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>285</v>
+        <v>206</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>320</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>60</v>
@@ -5453,19 +5687,19 @@
     </row>
     <row r="3" spans="1:6" ht="60">
       <c r="A3" s="21" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="E3" s="48" t="s">
-        <v>299</v>
+        <v>209</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>321</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>60</v>
@@ -5485,18 +5719,20 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G37" sqref="A1:XFD1048576"/>
+      <selection activeCell="J17" sqref="J17:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="53"/>
-    <col min="3" max="3" width="23" style="53" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="53"/>
-    <col min="6" max="6" width="13.85546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" style="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="2" width="9.140625" style="52"/>
+    <col min="3" max="3" width="23" style="52" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="52"/>
+    <col min="6" max="6" width="13.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="52"/>
+    <col min="11" max="11" width="33.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5524,16 +5760,16 @@
     </row>
     <row r="2" spans="1:7" ht="30">
       <c r="A2" s="18" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>12</v>
@@ -5541,8 +5777,8 @@
       <c r="F2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>308</v>
+      <c r="G2" s="17" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5559,20 +5795,20 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="A1:XFD1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="54"/>
-    <col min="3" max="3" width="37.42578125" style="53" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="53" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" style="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71" style="53" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="2" width="9.140625" style="53"/>
+    <col min="3" max="3" width="37.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51" style="52" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="54" customFormat="1">
+    <row r="1" spans="1:6" s="53" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>69</v>
       </c>
@@ -5589,103 +5825,103 @@
         <v>9</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="21" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>303</v>
+        <v>133</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>326</v>
       </c>
       <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="21" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>144</v>
+        <v>135</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>332</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="21" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>304</v>
+        <v>116</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>327</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="21" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>305</v>
+        <v>161</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>328</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="21" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E6" s="31"/>
-      <c r="F6" s="55" t="s">
-        <v>174</v>
+      <c r="F6" s="54" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>